<commit_message>
Basic Circuit Debug Work
</commit_message>
<xml_diff>
--- a/MorseCodeTranslater.xlsx
+++ b/MorseCodeTranslater.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cryst\Documents\School\CMPEN270Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6F84624C-B95A-4FF6-A3EA-695D407DBAE5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9D5AD396-D7EC-47F4-92D5-242F22780E4D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1" xr2:uid="{5AFDCA35-09A2-4749-AE54-30B0FB51A06B}"/>
   </bookViews>
@@ -274,9 +274,6 @@
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -321,6 +318,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -649,10 +649,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="21"/>
       <c r="D2" t="s">
         <v>30</v>
       </c>
@@ -670,11 +670,11 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="str">
+      <c r="C3" s="1" t="str">
         <f>_xlfn.BASE(B3,2,2)</f>
         <v>01</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E3" t="s">
@@ -683,7 +683,7 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="str">
+      <c r="G3" s="1" t="str">
         <f>_xlfn.BASE(F3,2,5)</f>
         <v>00000</v>
       </c>
@@ -692,7 +692,7 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="str">
+      <c r="C4" s="1" t="str">
         <f t="shared" ref="C4:C28" si="0">_xlfn.BASE(B4,2,2)</f>
         <v>10</v>
       </c>
@@ -705,7 +705,7 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" s="2" t="str">
+      <c r="G4" s="1" t="str">
         <f t="shared" ref="G4:G28" si="1">_xlfn.BASE(F4,2,5)</f>
         <v>00001</v>
       </c>
@@ -714,11 +714,11 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D5" s="2">
         <v>1010</v>
       </c>
       <c r="E5" t="s">
@@ -727,7 +727,7 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" s="2" t="str">
+      <c r="G5" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00010</v>
       </c>
@@ -736,7 +736,7 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="str">
+      <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -749,7 +749,7 @@
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="G6" s="2" t="str">
+      <c r="G6" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00011</v>
       </c>
@@ -758,7 +758,7 @@
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" s="2" t="str">
+      <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
@@ -771,7 +771,7 @@
       <c r="F7">
         <v>4</v>
       </c>
-      <c r="G7" s="2" t="str">
+      <c r="G7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00100</v>
       </c>
@@ -780,11 +780,11 @@
       <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E8" t="s">
@@ -793,7 +793,7 @@
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="G8" s="2" t="str">
+      <c r="G8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00101</v>
       </c>
@@ -802,7 +802,7 @@
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" s="2" t="str">
+      <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -815,7 +815,7 @@
       <c r="F9">
         <v>6</v>
       </c>
-      <c r="G9" s="2" t="str">
+      <c r="G9" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00110</v>
       </c>
@@ -824,11 +824,11 @@
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E10" t="s">
@@ -837,7 +837,7 @@
       <c r="F10">
         <v>7</v>
       </c>
-      <c r="G10" s="2" t="str">
+      <c r="G10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>00111</v>
       </c>
@@ -846,7 +846,7 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="2" t="str">
+      <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
@@ -859,7 +859,7 @@
       <c r="F11">
         <v>8</v>
       </c>
-      <c r="G11" s="2" t="str">
+      <c r="G11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>01000</v>
       </c>
@@ -868,11 +868,11 @@
       <c r="B12">
         <v>3</v>
       </c>
-      <c r="C12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E12" t="s">
@@ -881,7 +881,7 @@
       <c r="F12">
         <v>9</v>
       </c>
-      <c r="G12" s="2" t="str">
+      <c r="G12" s="1" t="str">
         <f t="shared" si="1"/>
         <v>01001</v>
       </c>
@@ -890,7 +890,7 @@
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" s="2" t="str">
+      <c r="C13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -903,7 +903,7 @@
       <c r="F13">
         <v>10</v>
       </c>
-      <c r="G13" s="2" t="str">
+      <c r="G13" s="1" t="str">
         <f t="shared" si="1"/>
         <v>01010</v>
       </c>
@@ -912,11 +912,11 @@
       <c r="B14">
         <v>3</v>
       </c>
-      <c r="C14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E14" t="s">
@@ -925,7 +925,7 @@
       <c r="F14">
         <v>11</v>
       </c>
-      <c r="G14" s="2" t="str">
+      <c r="G14" s="1" t="str">
         <f t="shared" si="1"/>
         <v>01011</v>
       </c>
@@ -934,7 +934,7 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="2" t="str">
+      <c r="C15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
@@ -947,7 +947,7 @@
       <c r="F15">
         <v>12</v>
       </c>
-      <c r="G15" s="2" t="str">
+      <c r="G15" s="1" t="str">
         <f t="shared" si="1"/>
         <v>01100</v>
       </c>
@@ -956,11 +956,11 @@
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="2" t="str">
+      <c r="C16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E16" t="s">
@@ -969,7 +969,7 @@
       <c r="F16">
         <v>13</v>
       </c>
-      <c r="G16" s="2" t="str">
+      <c r="G16" s="1" t="str">
         <f t="shared" si="1"/>
         <v>01101</v>
       </c>
@@ -978,7 +978,7 @@
       <c r="B17">
         <v>2</v>
       </c>
-      <c r="C17" s="2" t="str">
+      <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -991,7 +991,7 @@
       <c r="F17">
         <v>14</v>
       </c>
-      <c r="G17" s="2" t="str">
+      <c r="G17" s="1" t="str">
         <f t="shared" si="1"/>
         <v>01110</v>
       </c>
@@ -1000,11 +1000,11 @@
       <c r="B18">
         <v>3</v>
       </c>
-      <c r="C18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E18" t="s">
@@ -1013,7 +1013,7 @@
       <c r="F18">
         <v>15</v>
       </c>
-      <c r="G18" s="2" t="str">
+      <c r="G18" s="1" t="str">
         <f t="shared" si="1"/>
         <v>01111</v>
       </c>
@@ -1022,11 +1022,11 @@
       <c r="B19">
         <v>3</v>
       </c>
-      <c r="C19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D19" s="3">
+      <c r="C19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D19" s="2">
         <v>1101</v>
       </c>
       <c r="E19" t="s">
@@ -1035,7 +1035,7 @@
       <c r="F19">
         <v>16</v>
       </c>
-      <c r="G19" s="2" t="str">
+      <c r="G19" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10000</v>
       </c>
@@ -1044,11 +1044,11 @@
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20" s="2" t="str">
+      <c r="C20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E20" t="s">
@@ -1057,7 +1057,7 @@
       <c r="F20">
         <v>17</v>
       </c>
-      <c r="G20" s="2" t="str">
+      <c r="G20" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10001</v>
       </c>
@@ -1066,7 +1066,7 @@
       <c r="B21">
         <v>2</v>
       </c>
-      <c r="C21" s="2" t="str">
+      <c r="C21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1079,7 +1079,7 @@
       <c r="F21">
         <v>18</v>
       </c>
-      <c r="G21" s="2" t="str">
+      <c r="G21" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10010</v>
       </c>
@@ -1088,11 +1088,11 @@
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" s="2" t="str">
+      <c r="C22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E22" t="s">
@@ -1101,7 +1101,7 @@
       <c r="F22">
         <v>19</v>
       </c>
-      <c r="G22" s="2" t="str">
+      <c r="G22" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10011</v>
       </c>
@@ -1110,7 +1110,7 @@
       <c r="B23">
         <v>2</v>
       </c>
-      <c r="C23" s="2" t="str">
+      <c r="C23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1123,7 +1123,7 @@
       <c r="F23">
         <v>20</v>
       </c>
-      <c r="G23" s="2" t="str">
+      <c r="G23" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10100</v>
       </c>
@@ -1132,11 +1132,11 @@
       <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D24" s="5" t="s">
+      <c r="C24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>49</v>
       </c>
       <c r="E24" t="s">
@@ -1145,7 +1145,7 @@
       <c r="F24">
         <v>21</v>
       </c>
-      <c r="G24" s="2" t="str">
+      <c r="G24" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10101</v>
       </c>
@@ -1154,7 +1154,7 @@
       <c r="B25">
         <v>2</v>
       </c>
-      <c r="C25" s="2" t="str">
+      <c r="C25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1167,7 +1167,7 @@
       <c r="F25">
         <v>22</v>
       </c>
-      <c r="G25" s="2" t="str">
+      <c r="G25" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10110</v>
       </c>
@@ -1176,11 +1176,11 @@
       <c r="B26">
         <v>3</v>
       </c>
-      <c r="C26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D26" s="3">
+      <c r="C26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D26" s="2">
         <v>1001</v>
       </c>
       <c r="E26" t="s">
@@ -1189,7 +1189,7 @@
       <c r="F26">
         <v>23</v>
       </c>
-      <c r="G26" s="2" t="str">
+      <c r="G26" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10111</v>
       </c>
@@ -1198,11 +1198,11 @@
       <c r="B27">
         <v>3</v>
       </c>
-      <c r="C27" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D27" s="3">
+      <c r="C27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D27" s="2">
         <v>1011</v>
       </c>
       <c r="E27" t="s">
@@ -1211,7 +1211,7 @@
       <c r="F27">
         <v>24</v>
       </c>
-      <c r="G27" s="2" t="str">
+      <c r="G27" s="1" t="str">
         <f t="shared" si="1"/>
         <v>11000</v>
       </c>
@@ -1220,11 +1220,11 @@
       <c r="B28">
         <v>3</v>
       </c>
-      <c r="C28" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D28" s="3">
+      <c r="C28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D28" s="2">
         <v>1100</v>
       </c>
       <c r="E28" t="s">
@@ -1233,7 +1233,7 @@
       <c r="F28">
         <v>25</v>
       </c>
-      <c r="G28" s="2" t="str">
+      <c r="G28" s="1" t="str">
         <f t="shared" si="1"/>
         <v>11001</v>
       </c>
@@ -1251,7 +1251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF8C2CD-3391-4F0F-B3F6-C593087091BC}">
   <dimension ref="A2:I131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
@@ -1271,377 +1271,377 @@
       <c r="C2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>0</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>0</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>0</v>
       </c>
-      <c r="D3" s="11" t="str">
+      <c r="D3" s="10" t="str">
         <f>_xlfn.BASE(B3,2,2)</f>
         <v>00</v>
       </c>
-      <c r="E3" s="12" t="str">
+      <c r="E3" s="11" t="str">
         <f>_xlfn.BASE(C3,2,4)</f>
         <v>0000</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <f ca="1">COLUMN(INDIRECT(F3&amp;1))</f>
         <v>5</v>
       </c>
-      <c r="H3" s="11" t="str">
+      <c r="H3" s="10" t="str">
         <f ca="1">_xlfn.BASE(G3,2,5)</f>
         <v>00101</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>0</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>1</v>
       </c>
-      <c r="D4" s="11" t="str">
+      <c r="D4" s="10" t="str">
         <f t="shared" ref="D4:D66" si="0">_xlfn.BASE(B4,2,2)</f>
         <v>00</v>
       </c>
-      <c r="E4" s="12" t="str">
+      <c r="E4" s="11" t="str">
         <f t="shared" ref="E4:E66" si="1">_xlfn.BASE(C4,2,4)</f>
         <v>0001</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <f t="shared" ref="G4:G66" ca="1" si="2">COLUMN(INDIRECT(F4&amp;1))</f>
         <v>20</v>
       </c>
-      <c r="H4" s="11" t="str">
-        <f t="shared" ref="H4:H66" ca="1" si="3">_xlfn.BASE(G4,2,5)</f>
+      <c r="H4" s="10" t="str">
+        <f t="shared" ref="H4:H64" ca="1" si="3">_xlfn.BASE(G4,2,5)</f>
         <v>10100</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>0</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>2</v>
       </c>
-      <c r="D5" s="11" t="str">
+      <c r="D5" s="10" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E5" s="12" t="str">
+      <c r="E5" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0010</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
-      <c r="H5" s="11" t="str">
+      <c r="H5" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00101</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13">
-        <v>3</v>
-      </c>
-      <c r="B6" s="14">
+      <c r="A6" s="12">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13">
         <v>0</v>
       </c>
-      <c r="C6" s="13">
-        <v>3</v>
-      </c>
-      <c r="D6" s="14" t="str">
+      <c r="C6" s="12">
+        <v>3</v>
+      </c>
+      <c r="D6" s="13" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E6" s="15" t="str">
+      <c r="E6" s="14" t="str">
         <f t="shared" si="1"/>
         <v>0011</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
-      <c r="H6" s="14" t="str">
+      <c r="H6" s="13" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10100</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <v>4</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>0</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="16">
         <v>4</v>
       </c>
-      <c r="D7" s="17" t="str">
+      <c r="D7" s="16" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E7" s="18" t="str">
+      <c r="E7" s="17" t="str">
         <f t="shared" si="1"/>
         <v>0100</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
-      <c r="H7" s="17" t="str">
+      <c r="H7" s="16" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00101</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>5</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>0</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>5</v>
       </c>
-      <c r="D8" s="11" t="str">
+      <c r="D8" s="10" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E8" s="12" t="str">
+      <c r="E8" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0101</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
-      <c r="H8" s="11" t="str">
+      <c r="H8" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10100</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>0</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>6</v>
       </c>
-      <c r="D9" s="11" t="str">
+      <c r="D9" s="10" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E9" s="12" t="str">
+      <c r="E9" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0110</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
-      <c r="H9" s="11" t="str">
+      <c r="H9" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00101</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>7</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <v>0</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>7</v>
       </c>
-      <c r="D10" s="14" t="str">
+      <c r="D10" s="13" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E10" s="15" t="str">
+      <c r="E10" s="14" t="str">
         <f t="shared" si="1"/>
         <v>0111</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
-      <c r="H10" s="14" t="str">
+      <c r="H10" s="13" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10100</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
+      <c r="A11" s="15">
         <v>8</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>0</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="16">
         <v>8</v>
       </c>
-      <c r="D11" s="17" t="str">
+      <c r="D11" s="16" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E11" s="18" t="str">
+      <c r="E11" s="17" t="str">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="15">
         <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
-      <c r="H11" s="17" t="str">
+      <c r="H11" s="16" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00101</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>9</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>0</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>9</v>
       </c>
-      <c r="D12" s="11" t="str">
+      <c r="D12" s="10" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E12" s="12" t="str">
+      <c r="E12" s="11" t="str">
         <f t="shared" si="1"/>
         <v>1001</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
-      <c r="H12" s="11" t="str">
+      <c r="H12" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10100</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>10</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>0</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <v>10</v>
       </c>
-      <c r="D13" s="11" t="str">
+      <c r="D13" s="10" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E13" s="12" t="str">
+      <c r="E13" s="11" t="str">
         <f t="shared" si="1"/>
         <v>1010</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
-      <c r="H13" s="11" t="str">
+      <c r="H13" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00101</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13">
-        <v>11</v>
-      </c>
-      <c r="B14" s="14">
+      <c r="A14" s="12">
+        <v>11</v>
+      </c>
+      <c r="B14" s="13">
         <v>0</v>
       </c>
-      <c r="C14" s="13">
-        <v>11</v>
-      </c>
-      <c r="D14" s="14" t="str">
+      <c r="C14" s="12">
+        <v>11</v>
+      </c>
+      <c r="D14" s="13" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E14" s="15" t="str">
+      <c r="E14" s="14" t="str">
         <f t="shared" si="1"/>
         <v>1011</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="12">
         <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
-      <c r="H14" s="14" t="str">
+      <c r="H14" s="13" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10100</v>
       </c>
@@ -1650,17 +1650,17 @@
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>0</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>12</v>
       </c>
-      <c r="D15" s="2" t="str">
+      <c r="D15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E15" s="3" t="str">
+      <c r="E15" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1100</v>
       </c>
@@ -1671,7 +1671,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
-      <c r="H15" s="2" t="str">
+      <c r="H15" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00101</v>
       </c>
@@ -1680,17 +1680,17 @@
       <c r="A16">
         <v>13</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>0</v>
       </c>
       <c r="C16">
         <v>13</v>
       </c>
-      <c r="D16" s="2" t="str">
+      <c r="D16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E16" s="3" t="str">
+      <c r="E16" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1101</v>
       </c>
@@ -1701,7 +1701,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
-      <c r="H16" s="2" t="str">
+      <c r="H16" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10100</v>
       </c>
@@ -1710,17 +1710,17 @@
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>0</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>14</v>
       </c>
-      <c r="D17" s="2" t="str">
+      <c r="D17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E17" s="3" t="str">
+      <c r="E17" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1110</v>
       </c>
@@ -1731,397 +1731,397 @@
         <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
-      <c r="H17" s="2" t="str">
+      <c r="H17" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00101</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7">
+      <c r="A18" s="6">
         <v>15</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>0</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>15</v>
       </c>
-      <c r="D18" s="8" t="str">
+      <c r="D18" s="7" t="str">
         <f t="shared" si="0"/>
         <v>00</v>
       </c>
-      <c r="E18" s="9" t="str">
+      <c r="E18" s="8" t="str">
         <f t="shared" si="1"/>
         <v>1111</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
-      <c r="H18" s="8" t="str">
+      <c r="H18" s="7" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10100</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="19">
+      <c r="A19" s="18">
         <v>16</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="19">
         <v>1</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="19">
         <v>0</v>
       </c>
-      <c r="D19" s="20" t="str">
+      <c r="D19" s="19" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E19" s="21" t="str">
+      <c r="E19" s="20" t="str">
         <f t="shared" si="1"/>
         <v>0000</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="18">
         <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
-      <c r="H19" s="20" t="str">
+      <c r="H19" s="19" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01001</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="A20" s="9">
         <v>17</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <v>1</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>1</v>
       </c>
-      <c r="D20" s="11" t="str">
+      <c r="D20" s="10" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E20" s="12" t="str">
+      <c r="E20" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0001</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
-      <c r="H20" s="11" t="str">
+      <c r="H20" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00001</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="A21" s="9">
         <v>18</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="10">
         <v>1</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="10">
         <v>2</v>
       </c>
-      <c r="D21" s="11" t="str">
+      <c r="D21" s="10" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E21" s="12" t="str">
+      <c r="E21" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0010</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>14</v>
       </c>
-      <c r="H21" s="11" t="str">
+      <c r="H21" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01110</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13">
+      <c r="A22" s="12">
         <v>19</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="13">
         <v>1</v>
       </c>
-      <c r="C22" s="13">
-        <v>3</v>
-      </c>
-      <c r="D22" s="14" t="str">
+      <c r="C22" s="12">
+        <v>3</v>
+      </c>
+      <c r="D22" s="13" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E22" s="15" t="str">
+      <c r="E22" s="14" t="str">
         <f t="shared" si="1"/>
         <v>0011</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="12">
         <f t="shared" ca="1" si="2"/>
         <v>13</v>
       </c>
-      <c r="H22" s="14" t="str">
+      <c r="H22" s="13" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01101</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="16">
+      <c r="A23" s="15">
         <v>20</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="16">
         <v>1</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="16">
         <v>4</v>
       </c>
-      <c r="D23" s="17" t="str">
+      <c r="D23" s="16" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E23" s="18" t="str">
+      <c r="E23" s="17" t="str">
         <f t="shared" si="1"/>
         <v>0100</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="16">
+      <c r="G23" s="15">
         <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
-      <c r="H23" s="17" t="str">
+      <c r="H23" s="16" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01001</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="10">
+      <c r="A24" s="9">
         <v>21</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="10">
         <v>1</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="9">
         <v>5</v>
       </c>
-      <c r="D24" s="11" t="str">
+      <c r="D24" s="10" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E24" s="12" t="str">
+      <c r="E24" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0101</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
-      <c r="H24" s="11" t="str">
+      <c r="H24" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00001</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>22</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <v>1</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="10">
         <v>6</v>
       </c>
-      <c r="D25" s="11" t="str">
+      <c r="D25" s="10" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E25" s="12" t="str">
+      <c r="E25" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0110</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>14</v>
       </c>
-      <c r="H25" s="11" t="str">
+      <c r="H25" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01110</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="13">
+      <c r="A26" s="12">
         <v>23</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="13">
         <v>1</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="12">
         <v>7</v>
       </c>
-      <c r="D26" s="14" t="str">
+      <c r="D26" s="13" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E26" s="15" t="str">
+      <c r="E26" s="14" t="str">
         <f t="shared" si="1"/>
         <v>0111</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F26" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G26" s="12">
         <f t="shared" ca="1" si="2"/>
         <v>13</v>
       </c>
-      <c r="H26" s="14" t="str">
+      <c r="H26" s="13" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01101</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16">
+      <c r="A27" s="15">
         <v>24</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B27" s="16">
         <v>1</v>
       </c>
-      <c r="C27" s="17">
+      <c r="C27" s="16">
         <v>8</v>
       </c>
-      <c r="D27" s="17" t="str">
+      <c r="D27" s="16" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E27" s="18" t="str">
+      <c r="E27" s="17" t="str">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="16">
+      <c r="G27" s="15">
         <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
-      <c r="H27" s="17" t="str">
+      <c r="H27" s="16" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01001</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="10">
+      <c r="A28" s="9">
         <v>25</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="10">
         <v>1</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="9">
         <v>9</v>
       </c>
-      <c r="D28" s="11" t="str">
+      <c r="D28" s="10" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E28" s="12" t="str">
+      <c r="E28" s="11" t="str">
         <f t="shared" si="1"/>
         <v>1001</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
-      <c r="H28" s="11" t="str">
+      <c r="H28" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00001</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="10">
+      <c r="A29" s="9">
         <v>26</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B29" s="10">
         <v>1</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="10">
         <v>10</v>
       </c>
-      <c r="D29" s="11" t="str">
+      <c r="D29" s="10" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E29" s="12" t="str">
+      <c r="E29" s="11" t="str">
         <f t="shared" si="1"/>
         <v>1010</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>14</v>
       </c>
-      <c r="H29" s="11" t="str">
+      <c r="H29" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01110</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="13">
+      <c r="A30" s="12">
         <v>27</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="13">
         <v>1</v>
       </c>
-      <c r="C30" s="13">
-        <v>11</v>
-      </c>
-      <c r="D30" s="14" t="str">
+      <c r="C30" s="12">
+        <v>11</v>
+      </c>
+      <c r="D30" s="13" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E30" s="15" t="str">
+      <c r="E30" s="14" t="str">
         <f t="shared" si="1"/>
         <v>1011</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G30" s="12">
         <f t="shared" ca="1" si="2"/>
         <v>13</v>
       </c>
-      <c r="H30" s="14" t="str">
+      <c r="H30" s="13" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01101</v>
       </c>
@@ -2130,17 +2130,17 @@
       <c r="A31">
         <v>28</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>1</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>12</v>
       </c>
-      <c r="D31" s="2" t="str">
+      <c r="D31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E31" s="3" t="str">
+      <c r="E31" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1100</v>
       </c>
@@ -2151,7 +2151,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
-      <c r="H31" s="2" t="str">
+      <c r="H31" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01001</v>
       </c>
@@ -2160,17 +2160,17 @@
       <c r="A32">
         <v>29</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>1</v>
       </c>
       <c r="C32">
         <v>13</v>
       </c>
-      <c r="D32" s="2" t="str">
+      <c r="D32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E32" s="3" t="str">
+      <c r="E32" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1101</v>
       </c>
@@ -2181,7 +2181,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
-      <c r="H32" s="2" t="str">
+      <c r="H32" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00001</v>
       </c>
@@ -2190,17 +2190,17 @@
       <c r="A33">
         <v>30</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>1</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>14</v>
       </c>
-      <c r="D33" s="2" t="str">
+      <c r="D33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E33" s="3" t="str">
+      <c r="E33" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1110</v>
       </c>
@@ -2211,397 +2211,397 @@
         <f t="shared" ca="1" si="2"/>
         <v>14</v>
       </c>
-      <c r="H33" s="2" t="str">
+      <c r="H33" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01110</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="7">
+      <c r="A34" s="6">
         <v>31</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="7">
         <v>1</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <v>15</v>
       </c>
-      <c r="D34" s="8" t="str">
+      <c r="D34" s="7" t="str">
         <f t="shared" si="0"/>
         <v>01</v>
       </c>
-      <c r="E34" s="9" t="str">
+      <c r="E34" s="8" t="str">
         <f t="shared" si="1"/>
         <v>1111</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="6">
         <f t="shared" ca="1" si="2"/>
         <v>13</v>
       </c>
-      <c r="H34" s="8" t="str">
+      <c r="H34" s="7" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01101</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="19">
+      <c r="A35" s="18">
         <v>32</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="19">
         <v>2</v>
       </c>
-      <c r="C35" s="20">
+      <c r="C35" s="19">
         <v>0</v>
       </c>
-      <c r="D35" s="20" t="str">
+      <c r="D35" s="19" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E35" s="21" t="str">
+      <c r="E35" s="20" t="str">
         <f t="shared" si="1"/>
         <v>0000</v>
       </c>
-      <c r="F35" s="19" t="s">
+      <c r="F35" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G35" s="19">
+      <c r="G35" s="18">
         <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
-      <c r="H35" s="20" t="str">
+      <c r="H35" s="19" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10011</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="10">
+      <c r="A36" s="9">
         <v>33</v>
       </c>
-      <c r="B36" s="11">
+      <c r="B36" s="10">
         <v>2</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="9">
         <v>1</v>
       </c>
-      <c r="D36" s="11" t="str">
+      <c r="D36" s="10" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E36" s="12" t="str">
+      <c r="E36" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0001</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G36" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>21</v>
       </c>
-      <c r="H36" s="11" t="str">
+      <c r="H36" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10101</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="10">
+      <c r="A37" s="9">
         <v>34</v>
       </c>
-      <c r="B37" s="11">
+      <c r="B37" s="10">
         <v>2</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="10">
         <v>2</v>
       </c>
-      <c r="D37" s="11" t="str">
+      <c r="D37" s="10" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E37" s="12" t="str">
+      <c r="E37" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0010</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="10">
+      <c r="G37" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>18</v>
       </c>
-      <c r="H37" s="11" t="str">
+      <c r="H37" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10010</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="13">
+      <c r="A38" s="12">
         <v>35</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="13">
         <v>2</v>
       </c>
-      <c r="C38" s="13">
-        <v>3</v>
-      </c>
-      <c r="D38" s="14" t="str">
+      <c r="C38" s="12">
+        <v>3</v>
+      </c>
+      <c r="D38" s="13" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E38" s="15" t="str">
+      <c r="E38" s="14" t="str">
         <f t="shared" si="1"/>
         <v>0011</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="F38" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G38" s="13">
+      <c r="G38" s="12">
         <f t="shared" ca="1" si="2"/>
         <v>23</v>
       </c>
-      <c r="H38" s="14" t="str">
+      <c r="H38" s="13" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10111</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="16">
+      <c r="A39" s="15">
         <v>36</v>
       </c>
-      <c r="B39" s="17">
+      <c r="B39" s="16">
         <v>2</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="16">
         <v>4</v>
       </c>
-      <c r="D39" s="17" t="str">
+      <c r="D39" s="16" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E39" s="18" t="str">
+      <c r="E39" s="17" t="str">
         <f t="shared" si="1"/>
         <v>0100</v>
       </c>
-      <c r="F39" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39" s="16">
+      <c r="F39" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="15">
         <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
-      <c r="H39" s="17" t="str">
+      <c r="H39" s="16" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00100</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="10">
+      <c r="A40" s="9">
         <v>37</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B40" s="10">
         <v>2</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="9">
         <v>5</v>
       </c>
-      <c r="D40" s="11" t="str">
+      <c r="D40" s="10" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E40" s="12" t="str">
+      <c r="E40" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0101</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="F40" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G40" s="10">
-        <f t="shared" ca="1" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="H40" s="11" t="str">
+      <c r="G40" s="9">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="H40" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01011</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="10">
+      <c r="A41" s="9">
         <v>38</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B41" s="10">
         <v>2</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="10">
         <v>6</v>
       </c>
-      <c r="D41" s="11" t="str">
+      <c r="D41" s="10" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E41" s="12" t="str">
+      <c r="E41" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0110</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G41" s="10">
+      <c r="G41" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>7</v>
       </c>
-      <c r="H41" s="11" t="str">
+      <c r="H41" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00111</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="13">
+      <c r="A42" s="12">
         <v>39</v>
       </c>
-      <c r="B42" s="14">
+      <c r="B42" s="13">
         <v>2</v>
       </c>
-      <c r="C42" s="13">
+      <c r="C42" s="12">
         <v>7</v>
       </c>
-      <c r="D42" s="14" t="str">
+      <c r="D42" s="13" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E42" s="15" t="str">
+      <c r="E42" s="14" t="str">
         <f t="shared" si="1"/>
         <v>0111</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="13">
+      <c r="G42" s="12">
         <f t="shared" ca="1" si="2"/>
         <v>15</v>
       </c>
-      <c r="H42" s="14" t="str">
+      <c r="H42" s="13" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01111</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="16">
+      <c r="A43" s="15">
         <v>40</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B43" s="16">
         <v>2</v>
       </c>
-      <c r="C43" s="17">
+      <c r="C43" s="16">
         <v>8</v>
       </c>
-      <c r="D43" s="17" t="str">
+      <c r="D43" s="16" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E43" s="18" t="str">
+      <c r="E43" s="17" t="str">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="F43" s="16" t="s">
+      <c r="F43" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G43" s="16">
+      <c r="G43" s="15">
         <f t="shared" ca="1" si="2"/>
         <v>19</v>
       </c>
-      <c r="H43" s="17" t="str">
+      <c r="H43" s="16" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10011</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="10">
+      <c r="A44" s="9">
         <v>41</v>
       </c>
-      <c r="B44" s="11">
+      <c r="B44" s="10">
         <v>2</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="9">
         <v>9</v>
       </c>
-      <c r="D44" s="11" t="str">
+      <c r="D44" s="10" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E44" s="12" t="str">
+      <c r="E44" s="11" t="str">
         <f t="shared" si="1"/>
         <v>1001</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G44" s="10">
+      <c r="G44" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>21</v>
       </c>
-      <c r="H44" s="11" t="str">
+      <c r="H44" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10101</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="10">
+      <c r="A45" s="9">
         <v>42</v>
       </c>
-      <c r="B45" s="11">
+      <c r="B45" s="10">
         <v>2</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C45" s="10">
         <v>10</v>
       </c>
-      <c r="D45" s="11" t="str">
+      <c r="D45" s="10" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E45" s="12" t="str">
+      <c r="E45" s="11" t="str">
         <f t="shared" si="1"/>
         <v>1010</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F45" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G45" s="10">
+      <c r="G45" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>18</v>
       </c>
-      <c r="H45" s="11" t="str">
+      <c r="H45" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10010</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="13">
+      <c r="A46" s="12">
         <v>43</v>
       </c>
-      <c r="B46" s="14">
+      <c r="B46" s="13">
         <v>2</v>
       </c>
-      <c r="C46" s="13">
-        <v>11</v>
-      </c>
-      <c r="D46" s="14" t="str">
+      <c r="C46" s="12">
+        <v>11</v>
+      </c>
+      <c r="D46" s="13" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E46" s="15" t="str">
+      <c r="E46" s="14" t="str">
         <f t="shared" si="1"/>
         <v>1011</v>
       </c>
-      <c r="F46" s="13" t="s">
+      <c r="F46" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G46" s="13">
+      <c r="G46" s="12">
         <f t="shared" ca="1" si="2"/>
         <v>23</v>
       </c>
-      <c r="H46" s="14" t="str">
+      <c r="H46" s="13" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10111</v>
       </c>
@@ -2610,17 +2610,17 @@
       <c r="A47">
         <v>44</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>2</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <v>12</v>
       </c>
-      <c r="D47" s="2" t="str">
+      <c r="D47" s="1" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E47" s="3" t="str">
+      <c r="E47" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1100</v>
       </c>
@@ -2631,7 +2631,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
-      <c r="H47" s="2" t="str">
+      <c r="H47" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00100</v>
       </c>
@@ -2640,17 +2640,17 @@
       <c r="A48">
         <v>45</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>2</v>
       </c>
       <c r="C48">
         <v>13</v>
       </c>
-      <c r="D48" s="2" t="str">
+      <c r="D48" s="1" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E48" s="3" t="str">
+      <c r="E48" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1101</v>
       </c>
@@ -2661,7 +2661,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>11</v>
       </c>
-      <c r="H48" s="2" t="str">
+      <c r="H48" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01011</v>
       </c>
@@ -2670,17 +2670,17 @@
       <c r="A49">
         <v>46</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>2</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="1">
         <v>14</v>
       </c>
-      <c r="D49" s="2" t="str">
+      <c r="D49" s="1" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E49" s="3" t="str">
+      <c r="E49" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1110</v>
       </c>
@@ -2691,395 +2691,395 @@
         <f t="shared" ca="1" si="2"/>
         <v>7</v>
       </c>
-      <c r="H49" s="2" t="str">
+      <c r="H49" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00111</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="7">
+      <c r="A50" s="6">
         <v>47</v>
       </c>
-      <c r="B50" s="8">
+      <c r="B50" s="7">
         <v>2</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="6">
         <v>15</v>
       </c>
-      <c r="D50" s="8" t="str">
+      <c r="D50" s="7" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E50" s="9" t="str">
+      <c r="E50" s="8" t="str">
         <f t="shared" si="1"/>
         <v>1111</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="F50" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G50" s="7">
+      <c r="G50" s="6">
         <f t="shared" ca="1" si="2"/>
         <v>15</v>
       </c>
-      <c r="H50" s="8" t="str">
+      <c r="H50" s="7" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01111</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="19">
+      <c r="A51" s="18">
         <v>48</v>
       </c>
-      <c r="B51" s="20">
-        <v>3</v>
-      </c>
-      <c r="C51" s="20">
+      <c r="B51" s="19">
+        <v>3</v>
+      </c>
+      <c r="C51" s="19">
         <v>0</v>
       </c>
-      <c r="D51" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E51" s="21" t="str">
+      <c r="D51" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E51" s="20" t="str">
         <f t="shared" si="1"/>
         <v>0000</v>
       </c>
-      <c r="F51" s="19" t="s">
+      <c r="F51" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G51" s="19">
+      <c r="G51" s="18">
         <f t="shared" ca="1" si="2"/>
         <v>8</v>
       </c>
-      <c r="H51" s="20" t="str">
+      <c r="H51" s="19" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01000</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="10">
+      <c r="A52" s="9">
         <v>49</v>
       </c>
-      <c r="B52" s="11">
-        <v>3</v>
-      </c>
-      <c r="C52" s="10">
+      <c r="B52" s="10">
+        <v>3</v>
+      </c>
+      <c r="C52" s="9">
         <v>1</v>
       </c>
-      <c r="D52" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E52" s="12" t="str">
+      <c r="D52" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E52" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0001</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G52" s="10">
+      <c r="G52" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>22</v>
       </c>
-      <c r="H52" s="11" t="str">
+      <c r="H52" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10110</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="10">
+      <c r="A53" s="9">
         <v>50</v>
       </c>
-      <c r="B53" s="11">
-        <v>3</v>
-      </c>
-      <c r="C53" s="11">
+      <c r="B53" s="10">
+        <v>3</v>
+      </c>
+      <c r="C53" s="10">
         <v>2</v>
       </c>
-      <c r="D53" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E53" s="12" t="str">
+      <c r="D53" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E53" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0010</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G53" s="10">
+      <c r="G53" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
-      <c r="H53" s="11" t="str">
+      <c r="H53" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00110</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="13">
+      <c r="A54" s="12">
         <v>51</v>
       </c>
-      <c r="B54" s="14">
-        <v>3</v>
-      </c>
-      <c r="C54" s="13">
-        <v>3</v>
-      </c>
-      <c r="D54" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E54" s="15" t="str">
+      <c r="B54" s="13">
+        <v>3</v>
+      </c>
+      <c r="C54" s="12">
+        <v>3</v>
+      </c>
+      <c r="D54" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E54" s="14" t="str">
         <f t="shared" si="1"/>
         <v>0011</v>
       </c>
-      <c r="F54" s="13" t="s">
+      <c r="F54" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G54" s="13" t="e">
+      <c r="G54" s="12" t="e">
         <f t="shared" ca="1" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="H54" s="14" t="s">
+      <c r="H54" s="13" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="16">
+      <c r="A55" s="15">
         <v>52</v>
       </c>
-      <c r="B55" s="17">
-        <v>3</v>
-      </c>
-      <c r="C55" s="17">
+      <c r="B55" s="16">
+        <v>3</v>
+      </c>
+      <c r="C55" s="16">
         <v>4</v>
       </c>
-      <c r="D55" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E55" s="18" t="str">
+      <c r="D55" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E55" s="17" t="str">
         <f t="shared" si="1"/>
         <v>0100</v>
       </c>
-      <c r="F55" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" s="16">
+      <c r="F55" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="15">
         <f t="shared" ca="1" si="2"/>
         <v>12</v>
       </c>
-      <c r="H55" s="17" t="str">
+      <c r="H55" s="16" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01100</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="10">
+      <c r="A56" s="9">
         <v>53</v>
       </c>
-      <c r="B56" s="11">
-        <v>3</v>
-      </c>
-      <c r="C56" s="10">
+      <c r="B56" s="10">
+        <v>3</v>
+      </c>
+      <c r="C56" s="9">
         <v>5</v>
       </c>
-      <c r="D56" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E56" s="12" t="str">
+      <c r="D56" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E56" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0101</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G56" s="10" t="e">
+      <c r="G56" s="9" t="e">
         <f t="shared" ca="1" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="H56" s="11" t="s">
+      <c r="H56" s="10" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="10">
+      <c r="A57" s="9">
         <v>54</v>
       </c>
-      <c r="B57" s="11">
-        <v>3</v>
-      </c>
-      <c r="C57" s="11">
+      <c r="B57" s="10">
+        <v>3</v>
+      </c>
+      <c r="C57" s="10">
         <v>6</v>
       </c>
-      <c r="D57" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E57" s="12" t="str">
+      <c r="D57" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E57" s="11" t="str">
         <f t="shared" si="1"/>
         <v>0110</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G57" s="10">
+      <c r="G57" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>16</v>
       </c>
-      <c r="H57" s="11" t="str">
+      <c r="H57" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10000</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="13">
+      <c r="A58" s="12">
         <v>55</v>
       </c>
-      <c r="B58" s="14">
-        <v>3</v>
-      </c>
-      <c r="C58" s="13">
+      <c r="B58" s="13">
+        <v>3</v>
+      </c>
+      <c r="C58" s="12">
         <v>7</v>
       </c>
-      <c r="D58" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E58" s="15" t="str">
+      <c r="D58" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E58" s="14" t="str">
         <f t="shared" si="1"/>
         <v>0111</v>
       </c>
-      <c r="F58" s="13" t="s">
+      <c r="F58" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G58" s="13">
+      <c r="G58" s="12">
         <f t="shared" ca="1" si="2"/>
         <v>10</v>
       </c>
-      <c r="H58" s="14" t="str">
+      <c r="H58" s="13" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>01010</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="16">
+      <c r="A59" s="15">
         <v>56</v>
       </c>
-      <c r="B59" s="17">
-        <v>3</v>
-      </c>
-      <c r="C59" s="17">
+      <c r="B59" s="16">
+        <v>3</v>
+      </c>
+      <c r="C59" s="16">
         <v>8</v>
       </c>
-      <c r="D59" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E59" s="18" t="str">
+      <c r="D59" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E59" s="17" t="str">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="F59" s="16" t="s">
+      <c r="F59" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G59" s="16">
+      <c r="G59" s="15">
         <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
-      <c r="H59" s="17" t="str">
+      <c r="H59" s="16" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00010</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="10">
+      <c r="A60" s="9">
         <v>57</v>
       </c>
-      <c r="B60" s="11">
-        <v>3</v>
-      </c>
-      <c r="C60" s="10">
+      <c r="B60" s="10">
+        <v>3</v>
+      </c>
+      <c r="C60" s="9">
         <v>9</v>
       </c>
-      <c r="D60" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E60" s="12" t="str">
+      <c r="D60" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E60" s="11" t="str">
         <f t="shared" si="1"/>
         <v>1001</v>
       </c>
-      <c r="F60" s="10" t="s">
+      <c r="F60" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G60" s="10">
+      <c r="G60" s="9">
         <f t="shared" ca="1" si="2"/>
         <v>24</v>
       </c>
-      <c r="H60" s="11" t="str">
+      <c r="H60" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>11000</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="10">
+      <c r="A61" s="9">
         <v>58</v>
       </c>
-      <c r="B61" s="11">
-        <v>3</v>
-      </c>
-      <c r="C61" s="11">
+      <c r="B61" s="10">
+        <v>3</v>
+      </c>
+      <c r="C61" s="10">
         <v>10</v>
       </c>
-      <c r="D61" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E61" s="12" t="str">
+      <c r="D61" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E61" s="11" t="str">
         <f t="shared" si="1"/>
         <v>1010</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="F61" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G61" s="10">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="H61" s="11" t="str">
+      <c r="G61" s="9">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H61" s="10" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>00011</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="13">
+      <c r="A62" s="12">
         <v>59</v>
       </c>
-      <c r="B62" s="14">
-        <v>3</v>
-      </c>
-      <c r="C62" s="13">
-        <v>11</v>
-      </c>
-      <c r="D62" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E62" s="15" t="str">
+      <c r="B62" s="13">
+        <v>3</v>
+      </c>
+      <c r="C62" s="12">
+        <v>11</v>
+      </c>
+      <c r="D62" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E62" s="14" t="str">
         <f t="shared" si="1"/>
         <v>1011</v>
       </c>
-      <c r="F62" s="13" t="s">
+      <c r="F62" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G62" s="13">
+      <c r="G62" s="12">
         <f t="shared" ca="1" si="2"/>
         <v>25</v>
       </c>
-      <c r="H62" s="14" t="str">
+      <c r="H62" s="13" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>11001</v>
       </c>
@@ -3088,17 +3088,17 @@
       <c r="A63">
         <v>60</v>
       </c>
-      <c r="B63" s="2">
-        <v>3</v>
-      </c>
-      <c r="C63" s="2">
+      <c r="B63" s="1">
+        <v>3</v>
+      </c>
+      <c r="C63" s="1">
         <v>12</v>
       </c>
-      <c r="D63" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E63" s="3" t="str">
+      <c r="D63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E63" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1100</v>
       </c>
@@ -3109,7 +3109,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>26</v>
       </c>
-      <c r="H63" s="2" t="str">
+      <c r="H63" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>11010</v>
       </c>
@@ -3118,17 +3118,17 @@
       <c r="A64">
         <v>61</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>3</v>
       </c>
       <c r="C64">
         <v>13</v>
       </c>
-      <c r="D64" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E64" s="3" t="str">
+      <c r="D64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E64" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1101</v>
       </c>
@@ -3139,7 +3139,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>17</v>
       </c>
-      <c r="H64" s="2" t="str">
+      <c r="H64" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>10001</v>
       </c>
@@ -3148,17 +3148,17 @@
       <c r="A65">
         <v>62</v>
       </c>
-      <c r="B65" s="2">
-        <v>3</v>
-      </c>
-      <c r="C65" s="2">
+      <c r="B65" s="1">
+        <v>3</v>
+      </c>
+      <c r="C65" s="1">
         <v>14</v>
       </c>
-      <c r="D65" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E65" s="3" t="str">
+      <c r="D65" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E65" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1110</v>
       </c>
@@ -3169,7 +3169,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="H65" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3177,17 +3177,17 @@
       <c r="A66">
         <v>63</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="1">
         <v>3</v>
       </c>
       <c r="C66">
         <v>15</v>
       </c>
-      <c r="D66" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E66" s="3" t="str">
+      <c r="D66" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E66" s="2" t="str">
         <f t="shared" si="1"/>
         <v>1111</v>
       </c>
@@ -3198,204 +3198,204 @@
         <f t="shared" ca="1" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="H66" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D67" s="2"/>
+      <c r="D67" s="1"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D68" s="2"/>
+      <c r="D68" s="1"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D69" s="2"/>
+      <c r="D69" s="1"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D70" s="2"/>
+      <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D71" s="2"/>
+      <c r="D71" s="1"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D72" s="2"/>
+      <c r="D72" s="1"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D73" s="2"/>
+      <c r="D73" s="1"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D74" s="2"/>
+      <c r="D74" s="1"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D75" s="2"/>
+      <c r="D75" s="1"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D76" s="2"/>
+      <c r="D76" s="1"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D77" s="2"/>
+      <c r="D77" s="1"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D78" s="2"/>
+      <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D79" s="2"/>
+      <c r="D79" s="1"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D80" s="2"/>
+      <c r="D80" s="1"/>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D81" s="2"/>
+      <c r="D81" s="1"/>
     </row>
     <row r="82" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D82" s="2"/>
+      <c r="D82" s="1"/>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D83" s="2"/>
+      <c r="D83" s="1"/>
     </row>
     <row r="84" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D84" s="2"/>
+      <c r="D84" s="1"/>
     </row>
     <row r="85" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D85" s="2"/>
+      <c r="D85" s="1"/>
     </row>
     <row r="86" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D86" s="2"/>
+      <c r="D86" s="1"/>
     </row>
     <row r="87" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D87" s="2"/>
+      <c r="D87" s="1"/>
     </row>
     <row r="88" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D88" s="2"/>
+      <c r="D88" s="1"/>
     </row>
     <row r="89" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D89" s="2"/>
+      <c r="D89" s="1"/>
     </row>
     <row r="90" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D90" s="2"/>
+      <c r="D90" s="1"/>
     </row>
     <row r="91" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D91" s="2"/>
+      <c r="D91" s="1"/>
     </row>
     <row r="92" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D92" s="2"/>
+      <c r="D92" s="1"/>
     </row>
     <row r="93" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D93" s="2"/>
+      <c r="D93" s="1"/>
     </row>
     <row r="94" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D94" s="2"/>
+      <c r="D94" s="1"/>
     </row>
     <row r="95" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D95" s="2"/>
+      <c r="D95" s="1"/>
     </row>
     <row r="96" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D96" s="2"/>
+      <c r="D96" s="1"/>
     </row>
     <row r="97" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D97" s="2"/>
+      <c r="D97" s="1"/>
     </row>
     <row r="98" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D98" s="2"/>
+      <c r="D98" s="1"/>
     </row>
     <row r="99" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D99" s="2"/>
+      <c r="D99" s="1"/>
     </row>
     <row r="100" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D100" s="2"/>
+      <c r="D100" s="1"/>
     </row>
     <row r="101" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D101" s="2"/>
+      <c r="D101" s="1"/>
     </row>
     <row r="102" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D102" s="2"/>
+      <c r="D102" s="1"/>
     </row>
     <row r="103" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D103" s="2"/>
+      <c r="D103" s="1"/>
     </row>
     <row r="104" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D104" s="2"/>
+      <c r="D104" s="1"/>
     </row>
     <row r="105" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D105" s="2"/>
+      <c r="D105" s="1"/>
     </row>
     <row r="106" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D106" s="2"/>
+      <c r="D106" s="1"/>
     </row>
     <row r="107" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D107" s="2"/>
+      <c r="D107" s="1"/>
     </row>
     <row r="108" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D108" s="2"/>
+      <c r="D108" s="1"/>
     </row>
     <row r="109" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D109" s="2"/>
+      <c r="D109" s="1"/>
     </row>
     <row r="110" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D110" s="2"/>
+      <c r="D110" s="1"/>
     </row>
     <row r="111" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D111" s="2"/>
+      <c r="D111" s="1"/>
     </row>
     <row r="112" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D112" s="2"/>
+      <c r="D112" s="1"/>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D113" s="2"/>
+      <c r="D113" s="1"/>
     </row>
     <row r="114" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D114" s="2"/>
+      <c r="D114" s="1"/>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D115" s="2"/>
+      <c r="D115" s="1"/>
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D116" s="2"/>
+      <c r="D116" s="1"/>
     </row>
     <row r="117" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D117" s="2"/>
+      <c r="D117" s="1"/>
     </row>
     <row r="118" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D118" s="2"/>
+      <c r="D118" s="1"/>
     </row>
     <row r="119" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D119" s="2"/>
+      <c r="D119" s="1"/>
     </row>
     <row r="120" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D120" s="2"/>
+      <c r="D120" s="1"/>
     </row>
     <row r="121" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D121" s="2"/>
+      <c r="D121" s="1"/>
     </row>
     <row r="122" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D122" s="2"/>
+      <c r="D122" s="1"/>
     </row>
     <row r="123" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D123" s="2"/>
+      <c r="D123" s="1"/>
     </row>
     <row r="124" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D124" s="2"/>
+      <c r="D124" s="1"/>
     </row>
     <row r="125" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D125" s="2"/>
+      <c r="D125" s="1"/>
     </row>
     <row r="126" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D126" s="2"/>
+      <c r="D126" s="1"/>
     </row>
     <row r="127" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D127" s="2"/>
+      <c r="D127" s="1"/>
     </row>
     <row r="128" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D128" s="2"/>
+      <c r="D128" s="1"/>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D129" s="2"/>
+      <c r="D129" s="1"/>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D130" s="2"/>
+      <c r="D130" s="1"/>
     </row>
     <row r="131" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D131" s="2"/>
+      <c r="D131" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>